<commit_message>
add Use Item bug
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Equip.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Equip.xlsx
@@ -165,15 +165,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UI/SteampunkUI/resource/icons/img_equip.png</t>
-  </si>
-  <si>
     <t>EQUIP_ZS_M_0_ARMOR_10001</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>EQUIP_ZS_M_0_BOOT_10001</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI/SteampunkUI/resource/icons/img_equip</t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -668,7 +668,7 @@
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.75" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="47.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.15">
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
@@ -810,12 +810,12 @@
         <v>0</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.15">
@@ -902,12 +902,12 @@
         <v>0</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.15">
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
new tools(remove Aspose.Cells.dll, prefer to use NPOI, thanks @tangyu-1018); modify python interface(still error)
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/Equip.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/Equip.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\work\project\NFrame_CPP\_Out\Server\NFDataCfg\Excel_Ini\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="7905"/>
   </bookViews>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,10 +156,6 @@
   </si>
   <si>
     <t>Equip_Boot_102</t>
-  </si>
-  <si>
-    <t>s</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>皮革甲</t>
@@ -574,7 +575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -582,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -801,7 +802,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
@@ -910,11 +911,6 @@
       </c>
       <c r="O7">
         <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.15">
-      <c r="G19" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>